<commit_message>
position of bottom fix dot
</commit_message>
<xml_diff>
--- a/stimuli_en/multipleye-stimuli-practice-en.xlsx
+++ b/stimuli_en/multipleye-stimuli-practice-en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-image-creation/stimuli_en/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DF09BA-5965-514B-B83D-782CFDA30859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94E6AD4-94AB-5942-B281-AF98F75DEC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{CEBC6618-956B-204A-83A9-65FF22486C43}"/>
   </bookViews>
@@ -672,12 +672,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40A6B78-2830-0A44-97D8-ED183F8E9C4D}">
   <dimension ref="A1:AN13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q2" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="43.5" style="11" customWidth="1"/>
+    <col min="4" max="4" width="43.1640625" style="11" customWidth="1"/>
     <col min="21" max="26" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -803,7 +805,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:40" ht="289" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -919,7 +921,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:40" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:40" ht="221" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -929,7 +931,7 @@
       <c r="C3" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="11" t="s">
         <v>65</v>
       </c>
       <c r="E3" s="9"/>

</xml_diff>